<commit_message>
updated RAD test data
</commit_message>
<xml_diff>
--- a/RADTestData/PaymentsHardCoded.xlsx
+++ b/RADTestData/PaymentsHardCoded.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KatalonData\RADTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{A901629B-7390-4766-9C79-D73BA720F4D1}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1239D73A-CB02-4DFB-AD27-702C6F6B6E32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="15840" windowWidth="29040" xWindow="28680" xr2:uid="{DA3D39C3-C047-412A-8A87-CEDE42C5CB05}" yWindow="-120"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DA3D39C3-C047-412A-8A87-CEDE42C5CB05}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="83">
   <si>
     <t>Result</t>
   </si>
@@ -153,35 +153,142 @@
     <t>6011000993026909</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Pass</t>
   </si>
   <si>
-    <t>Thu Oct 28 17:22:24 EDT 2021</t>
-  </si>
-  <si>
-    <t>Thu Oct 28 17:28:42 EDT 2021</t>
-  </si>
-  <si>
-    <t>Thu Oct 28 17:42:39 EDT 2021</t>
-  </si>
-  <si>
-    <t>Thu Oct 28 17:43:26 EDT 2021</t>
-  </si>
-  <si>
-    <t>Thu Oct 28 17:44:18 EDT 2021</t>
-  </si>
-  <si>
-    <t>Thu Oct 28 17:45:03 EDT 2021</t>
+    <t>Thu Oct 28 21:24:16 EDT 2021</t>
+  </si>
+  <si>
+    <t>Thu Oct 28 21:25:06 EDT 2021</t>
+  </si>
+  <si>
+    <t>Thu Oct 28 21:25:58 EDT 2021</t>
+  </si>
+  <si>
+    <t>Personal Income Tax</t>
+  </si>
+  <si>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>Andrew</t>
+  </si>
+  <si>
+    <t>Larsons</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Cook</t>
+  </si>
+  <si>
+    <t>123450145</t>
+  </si>
+  <si>
+    <t>Bell</t>
+  </si>
+  <si>
+    <t>123459630</t>
+  </si>
+  <si>
+    <t>Vaughn</t>
+  </si>
+  <si>
+    <t>3652 Mandan road</t>
+  </si>
+  <si>
+    <t>114 Clark Ave</t>
+  </si>
+  <si>
+    <t>2000 14th street</t>
+  </si>
+  <si>
+    <t>Crofton</t>
+  </si>
+  <si>
+    <t>Severn</t>
+  </si>
+  <si>
+    <t>Columbia</t>
+  </si>
+  <si>
+    <t>21114</t>
+  </si>
+  <si>
+    <t>21144</t>
+  </si>
+  <si>
+    <t>21093</t>
+  </si>
+  <si>
+    <t>Fri Oct 29 15:41:33 EDT 2021</t>
+  </si>
+  <si>
+    <t>Fri Oct 29 15:42:24 EDT 2021</t>
+  </si>
+  <si>
+    <t>123452514</t>
+  </si>
+  <si>
+    <t>Fri Oct 29 15:51:19 EDT 2021</t>
+  </si>
+  <si>
+    <t>Extension Payments</t>
+  </si>
+  <si>
+    <t>Sales and Use</t>
+  </si>
+  <si>
+    <t>2022</t>
+  </si>
+  <si>
+    <t>January</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>December</t>
+  </si>
+  <si>
+    <t>My Glass Company</t>
+  </si>
+  <si>
+    <t>Superior, Painters</t>
+  </si>
+  <si>
+    <t>Light Car Wash</t>
+  </si>
+  <si>
+    <t>Withholding Tax</t>
+  </si>
+  <si>
+    <t>O'Briens Garage</t>
+  </si>
+  <si>
+    <t>A1 Tree Trimming</t>
+  </si>
+  <si>
+    <t>Lux &amp; Sons Corporation</t>
+  </si>
+  <si>
+    <t>O'Briens</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -224,28 +331,28 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -262,10 +369,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -300,7 +407,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -352,7 +459,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -463,21 +570,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -494,7 +601,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -546,42 +653,42 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB59299B-2CF9-4E8C-A692-AEB8ED0299FB}">
-  <dimension ref="A1:T5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB59299B-2CF9-4E8C-A692-AEB8ED0299FB}">
+  <dimension ref="A1:S22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="13.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="13.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="12.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="9.5703125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="10.140625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="4.7109375" collapsed="true"/>
-    <col min="20" max="16384" style="1" width="12.85546875" collapsed="true"/>
+    <col min="1" max="1" width="6.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="26.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="12.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="10.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="12" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="4.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="16384" width="12.85546875" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -645,13 +752,10 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
         <v>40</v>
-      </c>
-      <c r="B2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>19</v>
@@ -693,16 +797,14 @@
         <v>31</v>
       </c>
     </row>
-    <row customFormat="1" r="3" s="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>28</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="C3" s="4"/>
       <c r="D3" s="2" t="s">
         <v>19</v>
       </c>
@@ -743,16 +845,14 @@
         <v>31</v>
       </c>
     </row>
-    <row customFormat="1" r="4" s="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>28</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="C4" s="4"/>
       <c r="D4" s="3" t="s">
         <v>19</v>
       </c>
@@ -780,9 +880,6 @@
       <c r="N4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="Q4" s="3" t="s">
         <v>29</v>
       </c>
@@ -793,58 +890,744 @@
         <v>31</v>
       </c>
     </row>
-    <row customFormat="1" r="5" s="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="S5" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="H7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="O7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="Q7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="S7" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="S8" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="D9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="S9" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="D10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="S10" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="S11" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="D12" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="S12" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="C13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F13" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="S13" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="D14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="S14" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="D15" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="L5" s="3" t="s">
+      <c r="G15" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="S15" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="D16" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="L16" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R16" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="S16" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="4:19" ht="60" x14ac:dyDescent="0.25">
+      <c r="D17" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="L17" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="M17" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="N17" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="O17" s="4"/>
+      <c r="P17" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R17" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="S17" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="4:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="D18" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q18" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R18" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="S18" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="4:19" ht="30" x14ac:dyDescent="0.25">
+      <c r="D19" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q19" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R19" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="S19" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="4:19" s="4" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="D20" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="N20" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="P20" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="Q5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="R5" s="3" t="s">
+      <c r="Q20" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R20" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="S20" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="4:19" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="D21" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="M21" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="N21" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="P21" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q21" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R21" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="S21" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="4:19" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="D22" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="N22" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="P22" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q22" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R22" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="S5" s="3" t="s">
+      <c r="S22" s="4" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>